<commit_message>
rename folder, mod minigame
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skdiawotjd\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281B32B1-4705-41B5-992C-C18678B76AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -17,15 +18,16 @@
     <sheet name="설정" sheetId="5" r:id="rId3"/>
     <sheet name="분기점" sheetId="3" r:id="rId4"/>
     <sheet name="액티비티" sheetId="7" r:id="rId5"/>
-    <sheet name="계급표" sheetId="1" r:id="rId6"/>
-    <sheet name="스테이터스" sheetId="10" r:id="rId7"/>
-    <sheet name="직업트리" sheetId="6" r:id="rId8"/>
-    <sheet name="오브젝트" sheetId="8" r:id="rId9"/>
-    <sheet name="아이템" sheetId="11" r:id="rId10"/>
-    <sheet name="컨텐츠" sheetId="9" r:id="rId11"/>
-    <sheet name="Todo" sheetId="4" r:id="rId12"/>
-    <sheet name="씬" sheetId="12" r:id="rId13"/>
-    <sheet name="DDR" sheetId="14" r:id="rId14"/>
+    <sheet name="맵" sheetId="15" r:id="rId6"/>
+    <sheet name="컨텐츠" sheetId="9" r:id="rId7"/>
+    <sheet name="계급표" sheetId="1" r:id="rId8"/>
+    <sheet name="스테이터스" sheetId="10" r:id="rId9"/>
+    <sheet name="직업트리" sheetId="6" r:id="rId10"/>
+    <sheet name="오브젝트" sheetId="8" r:id="rId11"/>
+    <sheet name="아이템" sheetId="11" r:id="rId12"/>
+    <sheet name="Todo" sheetId="4" r:id="rId13"/>
+    <sheet name="씬" sheetId="12" r:id="rId14"/>
+    <sheet name="DDR" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="476">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2235,10 +2237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>귀족 스택이 +50~59</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>계급이 변경되면 나머지 값음 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2333,13 +2331,133 @@
   </si>
   <si>
     <t>준귀족1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀족 스택이 +50~99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넘버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이밍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미니rpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 노예(농사 및 채광)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 노예(청소)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 상인(판매)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddr - 노예(빨래)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddr - 명장(기술전수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddr - 대상인(기술전수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddr - 학자(연구성과시험)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이밍 - 대장장이(제작)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이밍 - 기사(위병활동)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아카데미 - (학문 수련)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방치형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2625,9 +2743,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2645,6 +2760,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2959,7 +3077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3184,7 +3302,439 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="54.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="18"/>
+    <col min="2" max="2" width="21.75" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3288,449 +3838,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="39"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" t="s">
-        <v>206</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>234</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>211</v>
-      </c>
-      <c r="B19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B20" t="s">
-        <v>214</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" s="39"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" s="39"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="D22" s="39"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>223</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="39"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B25" t="s">
-        <v>227</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>226</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>231</v>
-      </c>
-      <c r="B27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>325</v>
-      </c>
-      <c r="D27" s="39"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>230</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="D28" s="39"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>237</v>
-      </c>
-      <c r="B30" t="s">
-        <v>236</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>238</v>
-      </c>
-      <c r="D30" s="39"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>242</v>
-      </c>
-      <c r="B31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>243</v>
-      </c>
-      <c r="B32" t="s">
-        <v>245</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="D32" s="39"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>246</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="D33" s="39"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>244</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>249</v>
-      </c>
-      <c r="D34" s="39"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>261</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="D35" s="39"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>252</v>
-      </c>
-      <c r="B36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="D36" s="39"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>255</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="D37" s="39"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>261</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="D38" s="39"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>258</v>
-      </c>
-      <c r="B39" t="s">
-        <v>251</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="D39" s="39"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>259</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="D40" s="39"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>264</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>265</v>
-      </c>
-      <c r="D41" s="39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3795,8 +3904,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A9:C31"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -3908,8 +4017,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4066,7 +4175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4170,7 +4279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4292,11 +4401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4315,32 +4424,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>392</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>399</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="K1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>422</v>
-      </c>
-      <c r="M1" s="35" t="s">
+        <v>421</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>414</v>
       </c>
       <c r="O1" s="25" t="s">
         <v>393</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Q1" s="25" t="s">
         <v>413</v>
@@ -4375,16 +4484,16 @@
         <v>1</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>423</v>
-      </c>
-      <c r="M2" s="36" t="s">
+        <v>422</v>
+      </c>
+      <c r="M2" s="35" t="s">
         <v>415</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Q2" s="28">
         <v>1</v>
@@ -4416,19 +4525,19 @@
         <v>394</v>
       </c>
       <c r="K3" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="L3" s="29" t="s">
         <v>431</v>
       </c>
-      <c r="L3" s="29" t="s">
-        <v>432</v>
-      </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="35" t="s">
         <v>406</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q3" s="28">
         <v>50</v>
@@ -4463,16 +4572,16 @@
         <v>3</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>424</v>
-      </c>
-      <c r="M4" s="36" t="s">
+        <v>423</v>
+      </c>
+      <c r="M4" s="35" t="s">
         <v>405</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P4" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q4" s="28">
         <v>100</v>
@@ -4507,16 +4616,16 @@
         <v>13</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>425</v>
-      </c>
-      <c r="M5" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="M5" s="35" t="s">
         <v>403</v>
       </c>
       <c r="O5" s="30" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q5" s="28">
         <v>50</v>
@@ -4551,16 +4660,16 @@
         <v>14</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>426</v>
-      </c>
-      <c r="M6" s="36" t="s">
+        <v>425</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>404</v>
       </c>
       <c r="O6" s="30" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q6" s="28">
         <v>100</v>
@@ -4595,16 +4704,16 @@
         <v>69</v>
       </c>
       <c r="L7" s="30" t="s">
-        <v>433</v>
-      </c>
-      <c r="M7" s="36" t="s">
+        <v>432</v>
+      </c>
+      <c r="M7" s="35" t="s">
         <v>407</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P7" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Q7" s="28">
         <v>100</v>
@@ -4639,16 +4748,16 @@
         <v>71</v>
       </c>
       <c r="L8" s="30" t="s">
-        <v>427</v>
-      </c>
-      <c r="M8" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="M8" s="35" t="s">
         <v>408</v>
       </c>
       <c r="O8" s="31" t="s">
         <v>4</v>
       </c>
       <c r="P8" s="31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Q8" s="28">
         <v>100</v>
@@ -4683,9 +4792,9 @@
         <v>70</v>
       </c>
       <c r="L9" s="30" t="s">
-        <v>428</v>
-      </c>
-      <c r="M9" s="36" t="s">
+        <v>427</v>
+      </c>
+      <c r="M9" s="35" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4718,9 +4827,9 @@
         <v>72</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>429</v>
-      </c>
-      <c r="M10" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="M10" s="35" t="s">
         <v>410</v>
       </c>
     </row>
@@ -4753,9 +4862,9 @@
         <v>73</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="M11" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="M11" s="35" t="s">
         <v>416</v>
       </c>
     </row>
@@ -4788,9 +4897,9 @@
         <v>74</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="M12" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="M12" s="35" t="s">
         <v>417</v>
       </c>
     </row>
@@ -4823,9 +4932,9 @@
         <v>75</v>
       </c>
       <c r="L13" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="M13" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="M13" s="35" t="s">
         <v>418</v>
       </c>
     </row>
@@ -4858,9 +4967,9 @@
         <v>76</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="M14" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="M14" s="35" t="s">
         <v>419</v>
       </c>
     </row>
@@ -4893,10 +5002,10 @@
         <v>77</v>
       </c>
       <c r="L15" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="M15" s="36" t="s">
-        <v>420</v>
+        <v>429</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -4928,9 +5037,9 @@
         <v>78</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="M16" s="36" t="s">
+        <v>433</v>
+      </c>
+      <c r="M16" s="35" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4963,9 +5072,9 @@
         <v>4</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>435</v>
-      </c>
-      <c r="M17" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="M17" s="35" t="s">
         <v>412</v>
       </c>
     </row>
@@ -5008,38 +5117,8 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O22" s="24" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
+        <v>420</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5053,11 +5132,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5072,10 +5151,10 @@
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
@@ -5310,10 +5389,10 @@
       <c r="A17" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="1" t="s">
         <v>124</v>
       </c>
@@ -5526,11 +5605,1227 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B7D471-D188-4F11-95A1-CDF762171AFD}">
+  <dimension ref="A1:R33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>463</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>468</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="L1" s="40">
+        <v>10</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>447</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>448</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>450</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>452</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>451</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>475</v>
+      </c>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
+        <v>460</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40" t="s">
+        <v>456</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>471</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>473</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>453</v>
+      </c>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40" t="s">
+        <v>457</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>472</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40" t="s">
+        <v>454</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
+        <v>462</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40" t="s">
+        <v>458</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40" t="s">
+        <v>455</v>
+      </c>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>463</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40" t="s">
+        <v>459</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
+        <v>464</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
+        <v>468</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="38"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="38"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="38"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="38"/>
+    </row>
+    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="38"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" s="38"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="38"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="38"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="38"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="38"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="D25" s="38"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="38"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="D27" s="38"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>230</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="38"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="38"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D31" s="38"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" t="s">
+        <v>245</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" s="38"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" s="38"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>244</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" s="38"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="D35" s="38"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="D36" s="38"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>255</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="D37" s="38"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="38"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>258</v>
+      </c>
+      <c r="B39" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" s="38"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>259</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="38"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>264</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="D41" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B8" sqref="B8:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5916,8 +7211,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6041,436 +7336,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="54.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" style="18"/>
-    <col min="2" max="2" width="21.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="18"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>291</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add Home Scene, Range of Camera in accordance Background, order In Layer to Object
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skdiawotjd\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281B32B1-4705-41B5-992C-C18678B76AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -28,6 +27,7 @@
     <sheet name="Todo" sheetId="4" r:id="rId13"/>
     <sheet name="씬" sheetId="12" r:id="rId14"/>
     <sheet name="DDR" sheetId="14" r:id="rId15"/>
+    <sheet name="오브젝트 레이어 순서" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="480">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2453,11 +2453,27 @@
     <t>방치형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>배경화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무 등 상호작용이 불가능한 오브젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상호작용이 가능한 오브젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order In Layer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2749,6 +2765,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2760,9 +2779,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3077,7 +3093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3302,7 +3318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3676,7 +3692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3734,7 +3750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3839,7 +3855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3905,7 +3921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:C31"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -4018,7 +4034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4174,8 +4190,56 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4279,7 +4343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4401,7 +4465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4424,18 +4488,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>392</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="F1" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="K1" s="25" t="s">
         <v>0</v>
       </c>
@@ -5132,7 +5196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5151,10 +5215,10 @@
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
@@ -5389,10 +5453,10 @@
       <c r="A17" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="1" t="s">
         <v>124</v>
       </c>
@@ -5605,10 +5669,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B7D471-D188-4F11-95A1-CDF762171AFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -5622,756 +5686,756 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="36" t="s">
         <v>461</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="36" t="s">
         <v>462</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="36" t="s">
         <v>463</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="36" t="s">
         <v>465</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="36" t="s">
         <v>467</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="36" t="s">
         <v>468</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="36" t="s">
         <v>469</v>
       </c>
-      <c r="L1" s="40">
+      <c r="L1" s="36">
         <v>10</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="36" t="s">
         <v>474</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="36" t="s">
         <v>447</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="36" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="36" t="s">
         <v>450</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="36" t="s">
         <v>452</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="36" t="s">
         <v>451</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="36" t="s">
         <v>475</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>456</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="36" t="s">
         <v>471</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="36" t="s">
         <v>473</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="36" t="s">
         <v>461</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36" t="s">
         <v>457</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="36" t="s">
         <v>472</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="36" t="s">
         <v>454</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="36" t="s">
         <v>462</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36" t="s">
         <v>458</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
         <v>455</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="36" t="s">
         <v>463</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36" t="s">
         <v>459</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="36" t="s">
         <v>465</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="36" t="s">
         <v>467</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="36" t="s">
         <v>468</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="36" t="s">
         <v>469</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="36" t="s">
         <v>470</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="40"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="40"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="40"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="40"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="40"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6380,7 +6444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
@@ -6400,10 +6464,10 @@
       <c r="B1" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="38"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6412,10 +6476,10 @@
       <c r="B2" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -6424,10 +6488,10 @@
       <c r="B3" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6436,10 +6500,10 @@
       <c r="B4" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6448,10 +6512,10 @@
       <c r="B5" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="39"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6526,10 +6590,10 @@
       <c r="B14" t="s">
         <v>191</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="39"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -6538,19 +6602,19 @@
       <c r="B15" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="39"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="39"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -6559,8 +6623,8 @@
       <c r="B17" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -6569,10 +6633,10 @@
       <c r="B19" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="38"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -6581,10 +6645,10 @@
       <c r="B20" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="D20" s="38"/>
+      <c r="D20" s="39"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
@@ -6593,28 +6657,28 @@
       <c r="B21" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>222</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>223</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="39"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -6623,19 +6687,19 @@
       <c r="B25" t="s">
         <v>227</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="39"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>226</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="D26" s="38"/>
+      <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -6644,19 +6708,19 @@
       <c r="B27" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="38"/>
+      <c r="D27" s="39"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="D28" s="38"/>
+      <c r="D28" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -6665,10 +6729,10 @@
       <c r="B30" t="s">
         <v>236</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -6677,10 +6741,10 @@
       <c r="B31" t="s">
         <v>240</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="D31" s="38"/>
+      <c r="D31" s="39"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -6689,37 +6753,37 @@
       <c r="B32" t="s">
         <v>245</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="38"/>
+      <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>246</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="D33" s="38"/>
+      <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>244</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="D34" s="38"/>
+      <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>261</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="D35" s="38"/>
+      <c r="D35" s="39"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -6728,28 +6792,28 @@
       <c r="B36" t="s">
         <v>251</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="D36" s="38"/>
+      <c r="D36" s="39"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>255</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="39"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>261</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="D38" s="38"/>
+      <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -6758,38 +6822,42 @@
       <c r="B39" t="s">
         <v>251</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="D39" s="38"/>
+      <c r="D39" s="39"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>259</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D40" s="38"/>
+      <c r="D40" s="39"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>264</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="D41" s="38"/>
+      <c r="D41" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -6802,17 +6870,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6821,7 +6885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7212,7 +7276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add SceneLoadManager mod MainQuestManager mod MiniGameManager mod TownManager mod MiniGameNPC
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ED4067-AD67-4547-9CD4-4F557AACD437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C1980D-5892-450F-8262-896E0F641A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="465" windowWidth="17340" windowHeight="14010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="351">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1725,10 +1725,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ddr - 학자(연구성과시험)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1777,14 +1773,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>타이밍 - 기사(위병활동)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아카데미 - (학문 수련)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1813,10 +1801,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0205</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1833,19 +1817,147 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0205</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화 - 명장(타 국가 제작기술 배우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화 - 대상인(타 국가 제작기술 배우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집 - 노예</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운 - 노예</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집 - 상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집 - 대장장이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집 - 대상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집 - 명장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운 - 상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운 - 대장장이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운 - 대상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운 - 명장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건전달 - 노예(심부름)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건전달 - 대장장이(재료조달받기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건전달 - 상인(물품조달하기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀴즈 - 상인(판매기술배우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀴즈 - 대장장이(제작기술배우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0208</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가명장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가대상인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이밍 - 명장(제작)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 대상인(판매)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0305</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2018,7 +2130,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2136,6 +2248,9 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2147,12 +2262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2715,18 +2824,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="F1" s="39" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="K1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2912,10 +3021,10 @@
       <c r="M5" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="P5" s="44" t="s">
+      <c r="P5" s="39" t="s">
         <v>272</v>
       </c>
       <c r="Q5" s="25">
@@ -2956,10 +3065,10 @@
       <c r="M6" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="P6" s="44" t="s">
+      <c r="P6" s="39" t="s">
         <v>272</v>
       </c>
       <c r="Q6" s="25">
@@ -2991,10 +3100,10 @@
       <c r="I7" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="39" t="s">
         <v>265</v>
       </c>
       <c r="M7" s="32" t="s">
@@ -3011,7 +3120,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="39" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -3023,7 +3132,7 @@
       <c r="D8" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="39" t="s">
         <v>59</v>
       </c>
       <c r="G8" s="25" t="s">
@@ -3035,10 +3144,10 @@
       <c r="I8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="K8" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="39" t="s">
         <v>259</v>
       </c>
       <c r="M8" s="32" t="s">
@@ -3055,7 +3164,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -3067,7 +3176,7 @@
       <c r="D9" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="39" t="s">
         <v>61</v>
       </c>
       <c r="G9" s="25" t="s">
@@ -3079,10 +3188,10 @@
       <c r="I9" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="39" t="s">
         <v>260</v>
       </c>
       <c r="M9" s="32" t="s">
@@ -3090,7 +3199,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="39" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -3102,7 +3211,7 @@
       <c r="D10" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="39" t="s">
         <v>60</v>
       </c>
       <c r="G10" s="25" t="s">
@@ -3114,10 +3223,10 @@
       <c r="I10" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="39" t="s">
         <v>261</v>
       </c>
       <c r="M10" s="32" t="s">
@@ -3125,7 +3234,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="39" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -3137,7 +3246,7 @@
       <c r="D11" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="39" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="25" t="s">
@@ -3427,7 +3536,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3442,10 +3551,10 @@
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="40"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
@@ -3596,7 +3705,7 @@
       <c r="G10" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="2" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3686,10 +3795,10 @@
       <c r="A17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="1" t="s">
         <v>81</v>
       </c>
@@ -4093,7 +4202,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4109,10 +4218,10 @@
       <c r="B1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4121,10 +4230,10 @@
       <c r="B2" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4133,10 +4242,10 @@
       <c r="B3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4145,10 +4254,10 @@
       <c r="B4" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -4157,10 +4266,10 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -4235,10 +4344,10 @@
       <c r="B14" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4247,19 +4356,19 @@
       <c r="B15" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -4268,8 +4377,8 @@
       <c r="B17" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -4278,10 +4387,10 @@
       <c r="B19" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -4290,10 +4399,10 @@
       <c r="B20" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -4302,28 +4411,28 @@
       <c r="B21" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="42"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -4332,19 +4441,19 @@
       <c r="B25" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="42"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="42"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -4353,19 +4462,19 @@
       <c r="B27" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="42"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="41"/>
+      <c r="D28" s="42"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -4374,10 +4483,10 @@
       <c r="B30" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="42"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -4386,10 +4495,10 @@
       <c r="B31" t="s">
         <v>179</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -4398,37 +4507,37 @@
       <c r="B32" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="41"/>
+      <c r="D32" s="42"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="41"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="41"/>
+      <c r="D34" s="42"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="D35" s="41"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -4437,28 +4546,28 @@
       <c r="B36" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="D36" s="41"/>
+      <c r="D36" s="42"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>194</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="D37" s="41"/>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>200</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="41"/>
+      <c r="D38" s="42"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -4467,38 +4576,42 @@
       <c r="B39" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="41"/>
+      <c r="D39" s="42"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>198</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="41"/>
+      <c r="D40" s="42"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>203</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="D41" s="41"/>
+      <c r="D41" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -4511,17 +4624,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4533,58 +4642,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="33"/>
       <c r="B1" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="D1" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="L1" s="33">
-        <v>10</v>
-      </c>
       <c r="M1" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="N1" s="33"/>
+        <v>304</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>328</v>
+      </c>
       <c r="O1" s="33"/>
       <c r="P1" s="33"/>
       <c r="Q1" s="33"/>
@@ -4619,18 +4733,20 @@
         <v>284</v>
       </c>
       <c r="J2" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="K2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="M2" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="M2" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="N2" s="33"/>
+      <c r="N2" s="33" t="s">
+        <v>305</v>
+      </c>
       <c r="O2" s="33"/>
       <c r="P2" s="33"/>
       <c r="Q2" s="33"/>
@@ -4638,25 +4754,33 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+        <v>292</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>319</v>
+      </c>
       <c r="D3" s="33" t="s">
         <v>289</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="G3" s="33" t="s">
         <v>286</v>
       </c>
       <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="I3" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>330</v>
+      </c>
       <c r="K3" s="33"/>
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
@@ -4668,23 +4792,33 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+        <v>293</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>324</v>
+      </c>
       <c r="D4" s="33" t="s">
         <v>290</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>305</v>
-      </c>
-      <c r="F4" s="33"/>
+        <v>344</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>334</v>
+      </c>
       <c r="G4" s="33" t="s">
         <v>287</v>
       </c>
       <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="I4" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>332</v>
+      </c>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
@@ -4696,21 +4830,26 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>295</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+        <v>294</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>325</v>
+      </c>
       <c r="D5" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="E5" s="33"/>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="s">
         <v>288</v>
       </c>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="J5" s="33" t="s">
+        <v>331</v>
+      </c>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
@@ -4722,16 +4861,20 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
-        <v>292</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="D6" s="33"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="33" t="s">
+        <v>345</v>
+      </c>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
@@ -4746,10 +4889,14 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+        <v>296</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>327</v>
+      </c>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
@@ -4768,7 +4915,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -4790,7 +4937,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -4812,7 +4959,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -4834,7 +4981,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
@@ -4856,7 +5003,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
@@ -4878,7 +5025,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -5306,96 +5453,119 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="9" style="33"/>
     <col min="4" max="4" width="13.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="9" style="33"/>
-    <col min="14" max="14" width="11.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="33"/>
+    <col min="5" max="9" width="9" style="33"/>
+    <col min="10" max="10" width="11.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="9" style="33"/>
+    <col min="17" max="17" width="11.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>317</v>
-      </c>
       <c r="D1" s="36" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="J1" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="P1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="R1" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="S1" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="T1" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="U1" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>314</v>
+        <v>350</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+        <v>309</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>309</v>
+      </c>
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
       <c r="M2" s="34"/>
@@ -5404,26 +5574,41 @@
       <c r="P2" s="34"/>
       <c r="Q2" s="34"/>
       <c r="R2" s="34"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B3" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>322</v>
-      </c>
       <c r="D3" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+        <v>343</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>347</v>
+      </c>
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
@@ -5432,22 +5617,41 @@
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>316</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+        <v>335</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>348</v>
+      </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
@@ -5456,20 +5660,41 @@
       <c r="P4" s="34"/>
       <c r="Q4" s="34"/>
       <c r="R4" s="34"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+        <v>307</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>349</v>
+      </c>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
@@ -5478,10 +5703,15 @@
       <c r="P5" s="34"/>
       <c r="Q5" s="34"/>
       <c r="R5" s="34"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="B6" s="34" t="s">
+        <v>338</v>
+      </c>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -5498,10 +5728,15 @@
       <c r="P6" s="34"/>
       <c r="Q6" s="34"/>
       <c r="R6" s="34"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="B7" s="34" t="s">
+        <v>337</v>
+      </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -5518,10 +5753,15 @@
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="B8" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -5538,8 +5778,11 @@
       <c r="P8" s="34"/>
       <c r="Q8" s="34"/>
       <c r="R8" s="34"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -5558,8 +5801,11 @@
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -5578,8 +5824,11 @@
       <c r="P10" s="34"/>
       <c r="Q10" s="34"/>
       <c r="R10" s="34"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -5598,8 +5847,11 @@
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -5618,8 +5870,11 @@
       <c r="P12" s="34"/>
       <c r="Q12" s="34"/>
       <c r="R12" s="34"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="34"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -5638,8 +5893,11 @@
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -5658,8 +5916,11 @@
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
       <c r="R14" s="34"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -5678,8 +5939,11 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
@@ -5698,8 +5962,11 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -5718,8 +5985,11 @@
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -5738,6 +6008,9 @@
       <c r="P18" s="34"/>
       <c r="Q18" s="34"/>
       <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
bug fix of character
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C1980D-5892-450F-8262-896E0F641A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEF2F07-DEA5-48E2-B999-9823641B4A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="465" windowWidth="17340" windowHeight="14010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="352">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1958,6 +1958,10 @@
   </si>
   <si>
     <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인트로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2130,7 +2134,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2262,6 +2266,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2805,7 +2818,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A3" sqref="A3:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4601,17 +4614,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -4624,13 +4633,17 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4642,8 +4655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4659,44 +4672,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="34" t="s">
         <v>328</v>
       </c>
       <c r="O1" s="33"/>
@@ -4705,46 +4718,46 @@
       <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="34" t="s">
         <v>305</v>
       </c>
       <c r="O2" s="33"/>
@@ -4753,533 +4766,568 @@
       <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="45" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="45" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="46" t="s">
         <v>289</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>303</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="46" t="s">
         <v>286</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="J3" s="33" t="s">
+      <c r="H3" s="34"/>
+      <c r="I3" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="J3" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33"/>
       <c r="R3" s="33"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="45" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>290</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="45" t="s">
         <v>287</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="J4" s="33" t="s">
+      <c r="H4" s="34"/>
+      <c r="I4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
       <c r="O4" s="33"/>
       <c r="P4" s="33"/>
       <c r="Q4" s="33"/>
       <c r="R4" s="33"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33" t="s">
+      <c r="H5" s="34"/>
+      <c r="I5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
       <c r="Q5" s="33"/>
       <c r="R5" s="33"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="45" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
       <c r="O6" s="33"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="33"/>
       <c r="R6" s="33"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
       <c r="O7" s="33"/>
       <c r="P7" s="33"/>
       <c r="Q7" s="33"/>
       <c r="R7" s="33"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
       <c r="O8" s="33"/>
       <c r="P8" s="33"/>
       <c r="Q8" s="33"/>
       <c r="R8" s="33"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
       <c r="O9" s="33"/>
       <c r="P9" s="33"/>
       <c r="Q9" s="33"/>
       <c r="R9" s="33"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
       <c r="O10" s="33"/>
       <c r="P10" s="33"/>
       <c r="Q10" s="33"/>
       <c r="R10" s="33"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
       <c r="O11" s="33"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="33"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="33"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="33"/>
       <c r="R12" s="33"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
       <c r="O13" s="33"/>
       <c r="P13" s="33"/>
       <c r="Q13" s="33"/>
       <c r="R13" s="33"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="33"/>
       <c r="R14" s="33"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
       <c r="O15" s="33"/>
       <c r="P15" s="33"/>
       <c r="Q15" s="33"/>
       <c r="R15" s="33"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
       <c r="O16" s="33"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="33"/>
       <c r="R16" s="33"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
       <c r="O17" s="33"/>
       <c r="P17" s="33"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="33"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
       <c r="R18" s="33"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
       <c r="O19" s="33"/>
       <c r="P19" s="33"/>
       <c r="Q19" s="33"/>
       <c r="R19" s="33"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
       <c r="O20" s="33"/>
       <c r="P20" s="33"/>
       <c r="Q20" s="33"/>
       <c r="R20" s="33"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
       <c r="O21" s="33"/>
       <c r="P21" s="33"/>
       <c r="Q21" s="33"/>
       <c r="R21" s="33"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
       <c r="O22" s="33"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="33"/>
       <c r="R22" s="33"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
       <c r="O23" s="33"/>
       <c r="P23" s="33"/>
       <c r="Q23" s="33"/>
       <c r="R23" s="33"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
       <c r="Q24" s="33"/>
       <c r="R24" s="33"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
@@ -5455,7 +5503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mod Random.Range mod myPosition -> myMapNumber mod PlayerVector -> myPosition mod timing bar image
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skdiawotjd\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABA08F0-CA9F-4D10-B63F-77AD5D9A0B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="4"/>
+    <workbookView xWindow="6330" yWindow="1110" windowWidth="21495" windowHeight="14010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -1987,7 +1988,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2153,7 +2154,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2278,9 +2279,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2608,7 +2606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2833,7 +2831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2856,18 +2854,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="F1" s="43" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="K1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3564,7 +3562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3583,10 +3581,10 @@
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="44"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
@@ -3827,10 +3825,10 @@
       <c r="A17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="1" t="s">
         <v>81</v>
       </c>
@@ -4230,7 +4228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4250,10 +4248,10 @@
       <c r="B1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4262,10 +4260,10 @@
       <c r="B2" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4274,10 +4272,10 @@
       <c r="B3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4286,10 +4284,10 @@
       <c r="B4" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -4298,10 +4296,10 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -4376,10 +4374,10 @@
       <c r="B14" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4388,19 +4386,19 @@
       <c r="B15" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="45"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -4409,8 +4407,8 @@
       <c r="B17" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -4419,10 +4417,10 @@
       <c r="B19" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="44"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -4431,10 +4429,10 @@
       <c r="B20" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="45"/>
+      <c r="D20" s="44"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -4443,28 +4441,28 @@
       <c r="B21" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="44"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="D22" s="45"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="45"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -4473,19 +4471,19 @@
       <c r="B25" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="45"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="45"/>
+      <c r="D26" s="44"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -4494,19 +4492,19 @@
       <c r="B27" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="D27" s="45"/>
+      <c r="D27" s="44"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="44"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -4515,10 +4513,10 @@
       <c r="B30" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="45"/>
+      <c r="D30" s="44"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -4527,10 +4525,10 @@
       <c r="B31" t="s">
         <v>179</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="45"/>
+      <c r="D31" s="44"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -4539,37 +4537,37 @@
       <c r="B32" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="45"/>
+      <c r="D32" s="44"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="45"/>
+      <c r="D33" s="44"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="45"/>
+      <c r="D34" s="44"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="D35" s="45"/>
+      <c r="D35" s="44"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -4578,28 +4576,28 @@
       <c r="B36" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="D36" s="45"/>
+      <c r="D36" s="44"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>194</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="D37" s="45"/>
+      <c r="D37" s="44"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>200</v>
       </c>
-      <c r="C38" s="45" t="s">
+      <c r="C38" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="45"/>
+      <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -4608,28 +4606,28 @@
       <c r="B39" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="45"/>
+      <c r="D39" s="44"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>198</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="45"/>
+      <c r="D40" s="44"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>203</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="D41" s="45"/>
+      <c r="D41" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -4671,11 +4669,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4794,23 +4792,23 @@
       <c r="C3" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="41" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="41" t="s">
         <v>286</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="41" t="s">
         <v>330</v>
       </c>
       <c r="K3" s="34"/>
@@ -4826,19 +4824,19 @@
       <c r="A4" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="41" t="s">
         <v>320</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="41" t="s">
         <v>344</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="41" t="s">
         <v>334</v>
       </c>
       <c r="G4" s="41" t="s">
@@ -4848,7 +4846,7 @@
       <c r="I4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="41" t="s">
         <v>332</v>
       </c>
       <c r="K4" s="34"/>
@@ -4864,25 +4862,25 @@
       <c r="A5" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="41" t="s">
         <v>321</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="41" t="s">
         <v>291</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="34"/>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="41" t="s">
         <v>288</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="41" t="s">
         <v>331</v>
       </c>
       <c r="K5" s="34"/>
@@ -4898,7 +4896,7 @@
       <c r="A6" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="41" t="s">
         <v>322</v>
       </c>
       <c r="C6" s="41" t="s">
@@ -4907,7 +4905,7 @@
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="41" t="s">
         <v>345</v>
       </c>
       <c r="H6" s="34"/>
@@ -4928,7 +4926,7 @@
       <c r="A7" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="41" t="s">
         <v>323</v>
       </c>
       <c r="C7" s="41" t="s">
@@ -5529,7 +5527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6097,7 +6095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add MapNumber.csv mod arrow mod DDR,ObjectManager
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABA08F0-CA9F-4D10-B63F-77AD5D9A0B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C661A3-86FF-4B55-8F20-E0AC362E2A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="1110" windowWidth="21495" windowHeight="14010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="358">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1701,10 +1701,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오브젝트배치 - 노예(농사 및 채광)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오브젝트배치 - 노예(청소)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1982,6 +1978,14 @@
   </si>
   <si>
     <t>0400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 노예(농사)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트배치 - 노예(채광)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4631,13 +4635,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -4650,17 +4658,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4673,7 +4677,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4691,43 +4695,43 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
       <c r="B1" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>302</v>
-      </c>
       <c r="M1" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O1" s="33"/>
       <c r="P1" s="33"/>
@@ -4763,7 +4767,7 @@
         <v>284</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>132</v>
@@ -4775,7 +4779,7 @@
         <v>127</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O2" s="33"/>
       <c r="P2" s="33"/>
@@ -4784,32 +4788,32 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>319</v>
-      </c>
       <c r="D3" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>286</v>
+        <v>357</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
@@ -4822,32 +4826,32 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="40" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -4860,28 +4864,28 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="34"/>
       <c r="G5" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="40" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
@@ -4894,19 +4898,19 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
       <c r="G6" s="41" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="40" t="s">
@@ -4924,18 +4928,20 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="34" t="s">
+        <v>356</v>
+      </c>
       <c r="H7" s="34"/>
       <c r="I7" s="40" t="s">
         <v>13</v>
@@ -4952,7 +4958,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
@@ -4976,7 +4982,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -5000,7 +5006,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -5024,7 +5030,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -5048,7 +5054,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -5072,7 +5078,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -5236,7 +5242,7 @@
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -5258,7 +5264,7 @@
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
       <c r="I21" s="34" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
@@ -5373,7 +5379,7 @@
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
       <c r="B27" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
@@ -5395,7 +5401,7 @@
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
       <c r="B28" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -5417,7 +5423,7 @@
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
       <c r="B29" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
@@ -5439,7 +5445,7 @@
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
       <c r="B30" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -5461,7 +5467,7 @@
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
       <c r="B31" s="33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
@@ -5550,31 +5556,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C1" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>313</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>314</v>
       </c>
       <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>59</v>
@@ -5612,34 +5618,34 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
@@ -5655,34 +5661,34 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
@@ -5698,34 +5704,34 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -5741,34 +5747,34 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
@@ -5785,7 +5791,7 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
@@ -5810,7 +5816,7 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -5835,7 +5841,7 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>

</xml_diff>

<commit_message>
add PortalNameList.csv mod MiniGameNPC.cs
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EF091E-3057-48E9-AC19-E4EB6C871624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D343D-D140-4262-AE31-0ADD3D42F427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="930" windowWidth="21495" windowHeight="14010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="1440" windowWidth="21495" windowHeight="14010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="432">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1750,6 +1750,26 @@
   </si>
   <si>
     <t>노예 모험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평민 타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>준귀족 타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀족 타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕 타운</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2065,6 +2085,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2084,9 +2107,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3025,14 +3045,14 @@
       <c r="B1" s="37" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
       <c r="I1" s="37" t="s">
         <v>288</v>
       </c>
@@ -3216,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF524D-E86E-4617-8759-56910C557665}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3231,7 +3251,7 @@
     <col min="10" max="11" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="30" t="s">
         <v>205</v>
@@ -3272,8 +3292,11 @@
       <c r="N1" s="30" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>201</v>
       </c>
@@ -3316,8 +3339,11 @@
       <c r="N2" s="30" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="50" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>205</v>
       </c>
@@ -3341,17 +3367,20 @@
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="49" t="s">
+      <c r="J3" s="43" t="s">
         <v>425</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="K3" s="43" t="s">
         <v>426</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>206</v>
       </c>
@@ -3382,8 +3411,11 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>207</v>
       </c>
@@ -3395,23 +3427,26 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="30" t="s">
         <v>394</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="30" t="s">
         <v>397</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="30" t="s">
         <v>396</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>208</v>
       </c>
@@ -3432,8 +3467,11 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>209</v>
       </c>
@@ -3453,7 +3491,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>210</v>
       </c>
@@ -3471,7 +3509,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>211</v>
       </c>
@@ -3489,7 +3527,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>212</v>
       </c>
@@ -3507,7 +3545,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>213</v>
       </c>
@@ -3525,7 +3563,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>214</v>
       </c>
@@ -3543,7 +3581,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>215</v>
       </c>
@@ -3561,7 +3599,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3577,7 +3615,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3593,7 +3631,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -4063,19 +4101,19 @@
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>354</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -4478,10 +4516,10 @@
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
@@ -4722,10 +4760,10 @@
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="1" t="s">
         <v>54</v>
       </c>
@@ -5145,10 +5183,10 @@
       <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5157,10 +5195,10 @@
       <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="48"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5169,10 +5207,10 @@
       <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5181,10 +5219,10 @@
       <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -5193,10 +5231,10 @@
       <c r="B5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5271,10 +5309,10 @@
       <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="48"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -5283,19 +5321,19 @@
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="48"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="47"/>
+      <c r="D16" s="48"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -5304,8 +5342,8 @@
       <c r="B17" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -5314,10 +5352,10 @@
       <c r="B19" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -5326,10 +5364,10 @@
       <c r="B20" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -5338,28 +5376,28 @@
       <c r="B21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -5368,19 +5406,19 @@
       <c r="B25" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -5389,19 +5427,19 @@
       <c r="B27" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -5410,10 +5448,10 @@
       <c r="B30" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -5422,10 +5460,10 @@
       <c r="B31" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -5434,37 +5472,37 @@
       <c r="B32" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -5473,28 +5511,28 @@
       <c r="B36" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -5503,38 +5541,42 @@
       <c r="B39" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>170</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -5547,17 +5589,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add QuestGiveNpc.cs add ManufactureRecipe.csv add QuestUI
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D343D-D140-4262-AE31-0ADD3D42F427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A402B-DB31-428C-AF58-43D1F117B8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="1440" windowWidth="21495" windowHeight="14010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="1440" windowWidth="21495" windowHeight="14010" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="444">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1729,10 +1729,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>반복</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>게임반복</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1770,6 +1766,58 @@
   </si>
   <si>
     <t>왕 타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>04xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>06xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복퀘스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템반복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9xxx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1955,7 +2003,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2105,9 +2153,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3238,7 +3283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF524D-E86E-4617-8759-56910C557665}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -3339,8 +3384,8 @@
       <c r="N2" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="O2" s="50" t="s">
-        <v>427</v>
+      <c r="O2" s="43" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3368,16 +3413,16 @@
       <c r="H3" s="30"/>
       <c r="I3" s="2"/>
       <c r="J3" s="43" t="s">
+        <v>424</v>
+      </c>
+      <c r="K3" s="43" t="s">
         <v>425</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>426</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
       <c r="O3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3412,7 +3457,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3443,7 +3488,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3468,7 +3513,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3799,10 +3844,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A26"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3829,245 +3874,306 @@
         <v>421</v>
       </c>
       <c r="D2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>420</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>431</v>
+      </c>
+      <c r="D5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>432</v>
+      </c>
+      <c r="D6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D9" t="s">
+        <v>441</v>
+      </c>
+      <c r="E9" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E10" t="s">
         <v>423</v>
       </c>
-      <c r="E3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>299</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>308</v>
-      </c>
-      <c r="D4" t="s">
-        <v>306</v>
-      </c>
-      <c r="E4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>300</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="D5" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>310</v>
-      </c>
-      <c r="D6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="D7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
-        <v>314</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="B10" s="29"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="B11" s="29"/>
+      <c r="A11" t="s">
+        <v>437</v>
+      </c>
+      <c r="D11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E11" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="B12" s="29"/>
+        <v>299</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>318</v>
-      </c>
-      <c r="B13" s="29"/>
+        <v>300</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>328</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="B18" s="29"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>330</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>337</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="B19" s="29"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B20" s="29"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>332</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="B21" s="29"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>333</v>
+        <v>319</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>334</v>
+        <v>322</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>335</v>
-      </c>
-      <c r="B24" t="s">
-        <v>340</v>
+        <v>323</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="B25" t="s">
-        <v>352</v>
+        <v>325</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>342</v>
+        <v>327</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
-        <v>343</v>
+        <v>330</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>344</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="B28" s="29"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="B32" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="B33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="29" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="29" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="29" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="29" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="29" t="s">
         <v>351</v>
       </c>
     </row>
@@ -4082,7 +4188,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4364,8 +4470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5566,17 +5672,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -5589,13 +5691,17 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mod SceneLoadManager mod QuizManager mod word,excel mod DNFBitBit/DNFBitBitTTF SDF.asset
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54476D32-78B8-4911-814C-3AADE9ED6348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477CF5A0-092B-44CC-96B5-6999CD7E77AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="449">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1127,10 +1127,6 @@
   </si>
   <si>
     <t>퀴즈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DDR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2033,7 +2029,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2166,6 +2162,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2183,12 +2182,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2496,7 +2489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2891,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2931,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>245</v>
@@ -2940,7 +2933,7 @@
         <v>252</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G2" s="23">
         <v>50</v>
@@ -2954,13 +2947,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>245</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>200</v>
@@ -2977,7 +2970,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>245</v>
@@ -2986,7 +2979,7 @@
         <v>251</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G4" s="23">
         <v>50</v>
@@ -3000,7 +2993,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>253</v>
@@ -3015,24 +3008,24 @@
         <v>50</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>280</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>281</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>250</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G6" s="23">
         <v>50</v>
@@ -3046,7 +3039,7 @@
         <v>248</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>254</v>
@@ -3066,16 +3059,16 @@
         <v>249</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="51" t="s">
-        <v>447</v>
+      <c r="F8" s="44" t="s">
+        <v>446</v>
       </c>
       <c r="G8" s="23">
         <v>50</v>
@@ -3086,16 +3079,16 @@
         <v>250</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="E9" s="51" t="s">
-        <v>446</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>448</v>
+      <c r="E9" s="44" t="s">
+        <v>445</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>447</v>
       </c>
       <c r="G9" s="23">
         <v>100</v>
@@ -3106,16 +3099,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>449</v>
+      <c r="F10" s="44" t="s">
+        <v>448</v>
       </c>
       <c r="G10" s="23">
         <v>100</v>
@@ -3132,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3151,21 +3144,21 @@
         <v>264</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="37" t="s">
-        <v>288</v>
-      </c>
       <c r="J1" s="37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3188,11 +3181,11 @@
         <v>268</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>269</v>
+        <v>178</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J2" s="39"/>
     </row>
@@ -3201,26 +3194,26 @@
         <v>3</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>263</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>107</v>
       </c>
       <c r="F3" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" s="39" t="s">
         <v>271</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>272</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J3" s="39"/>
     </row>
@@ -3229,13 +3222,13 @@
         <v>34</v>
       </c>
       <c r="B4" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="39" t="s">
         <v>274</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>275</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>266</v>
@@ -3247,18 +3240,18 @@
         <v>178</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>262</v>
@@ -3267,55 +3260,55 @@
         <v>267</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>266</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>178</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D6" s="39" t="s">
         <v>267</v>
       </c>
       <c r="E6" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>283</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>284</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>178</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3412,7 +3405,7 @@
         <v>202</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>204</v>
@@ -3448,7 +3441,7 @@
         <v>217</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3456,36 +3449,36 @@
         <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D3" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="F3" s="30" t="s">
         <v>378</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>379</v>
-      </c>
       <c r="G3" s="30" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="2"/>
       <c r="J3" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="K3" s="43" t="s">
         <v>424</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>425</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
       <c r="O3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3493,36 +3486,36 @@
         <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D4" s="50" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
       <c r="J4" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="K4" s="30" t="s">
         <v>380</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>381</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3530,7 +3523,7 @@
         <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>100</v>
@@ -3540,22 +3533,22 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="30" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K5" s="30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3563,10 +3556,10 @@
         <v>208</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
@@ -3582,7 +3575,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3591,7 +3584,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
@@ -3654,7 +3647,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3930,329 +3923,329 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" t="s">
         <v>297</v>
       </c>
-      <c r="B1" t="s">
-        <v>298</v>
-      </c>
       <c r="D1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" t="s">
         <v>304</v>
-      </c>
-      <c r="E1" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E2" t="s">
         <v>438</v>
-      </c>
-      <c r="E2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" t="s">
         <v>306</v>
-      </c>
-      <c r="E3" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E5" t="s">
         <v>338</v>
-      </c>
-      <c r="E5" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B19" s="29"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" s="29"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B21" s="29"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B25" s="29" t="s">
         <v>325</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>327</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B28" s="29"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4285,33 +4278,33 @@
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>357</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>358</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -4324,12 +4317,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -4342,12 +4335,12 @@
         <v>34</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
@@ -4357,15 +4350,15 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
@@ -4375,7 +4368,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -4561,39 +4554,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>409</v>
-      </c>
       <c r="C1" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>406</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>407</v>
-      </c>
       <c r="G1" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>416</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>400</v>
-      </c>
       <c r="D2" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -4601,47 +4594,47 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>401</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>416</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>402</v>
       </c>
       <c r="D3" s="29">
         <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D4" s="29">
         <v>4</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D5" s="29">
         <v>5</v>
@@ -4700,10 +4693,10 @@
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="47"/>
+      <c r="C1" s="48"/>
       <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
@@ -4944,10 +4937,10 @@
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="47"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="1" t="s">
         <v>54</v>
       </c>
@@ -5367,10 +5360,10 @@
       <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="48"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5379,10 +5372,10 @@
       <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5391,10 +5384,10 @@
       <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5403,10 +5396,10 @@
       <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -5415,10 +5408,10 @@
       <c r="B5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5493,10 +5486,10 @@
       <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="49"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -5505,19 +5498,19 @@
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -5526,8 +5519,8 @@
       <c r="B17" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -5536,10 +5529,10 @@
       <c r="B19" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -5548,10 +5541,10 @@
       <c r="B20" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="48"/>
+      <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -5560,28 +5553,28 @@
       <c r="B21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="48"/>
+      <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="48"/>
+      <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="49"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -5590,19 +5583,19 @@
       <c r="B25" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="49"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="49"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -5611,19 +5604,19 @@
       <c r="B27" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="49"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -5632,10 +5625,10 @@
       <c r="B30" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="48"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -5644,10 +5637,10 @@
       <c r="B31" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="48"/>
+      <c r="D31" s="49"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -5656,37 +5649,37 @@
       <c r="B32" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="48"/>
+      <c r="D32" s="49"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="D33" s="48"/>
+      <c r="D33" s="49"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="48"/>
+      <c r="D34" s="49"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="48"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -5695,28 +5688,28 @@
       <c r="B36" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="48"/>
+      <c r="D36" s="49"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="48"/>
+      <c r="D37" s="49"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="D38" s="49"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -5725,38 +5718,42 @@
       <c r="B39" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="48"/>
+      <c r="D39" s="49"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>170</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="48"/>
+      <c r="D40" s="49"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="48" t="s">
+      <c r="C41" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="48"/>
+      <c r="D41" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -5769,17 +5766,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mod QuestManager mod TutorialManager mod ExploreManager add ExploreSelectFloatingMessage.csv
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477CF5A0-092B-44CC-96B5-6999CD7E77AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A2A938-4ADA-404B-B9DE-03266B4CF8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="1875" windowWidth="17025" windowHeight="12675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="450">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1838,6 +1838,10 @@
   </si>
   <si>
     <t>_myStackByJob[8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노예 주조</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3125,7 +3129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3339,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF524D-E86E-4617-8759-56910C557665}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3457,8 +3461,8 @@
       <c r="D3" s="30" t="s">
         <v>377</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>391</v>
+      <c r="E3" t="s">
+        <v>449</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>378</v>
@@ -3495,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>397</v>
@@ -3531,7 +3535,9 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="30" t="s">
+        <v>394</v>
+      </c>
       <c r="F5" s="30" t="s">
         <v>393</v>
       </c>
@@ -5743,17 +5749,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -5766,13 +5768,17 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mod adventure logic mod explore playerAttack, EnemyAttack
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A2A938-4ADA-404B-B9DE-03266B4CF8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBDFED8-75F2-45E4-9FD2-75C7C70ED619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="1875" windowWidth="17025" windowHeight="12675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="컨텐츠" sheetId="19" r:id="rId3"/>
     <sheet name="맵" sheetId="22" r:id="rId4"/>
     <sheet name="오브젝트" sheetId="20" r:id="rId5"/>
-    <sheet name="퀘스트" sheetId="17" r:id="rId6"/>
-    <sheet name="퀘스트넘버" sheetId="21" r:id="rId7"/>
-    <sheet name="액티비티" sheetId="7" r:id="rId8"/>
-    <sheet name="컨텐츠1" sheetId="9" r:id="rId9"/>
-    <sheet name="난이도" sheetId="14" r:id="rId10"/>
+    <sheet name="아이템" sheetId="23" r:id="rId6"/>
+    <sheet name="퀘스트" sheetId="17" r:id="rId7"/>
+    <sheet name="퀘스트넘버" sheetId="21" r:id="rId8"/>
+    <sheet name="액티비티" sheetId="7" r:id="rId9"/>
+    <sheet name="컨텐츠1" sheetId="9" r:id="rId10"/>
+    <sheet name="난이도" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="459">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1114,78 +1115,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>모험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위병</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>의뢰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Timing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의뢰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀴즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연금술사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연금술사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연금술사 스택이 0~50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방치형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>모험</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>탐험</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>퀴즈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탐험</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>타이밍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DDR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탐험</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위병</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의뢰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Timing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의뢰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>퀴즈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연금술사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연금술사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연금술사 스택이 0~50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방치형</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모험</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>제작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1486,10 +1471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>의뢰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>재료 얻기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1842,6 +1823,62 @@
   </si>
   <si>
     <t>노예 주조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDR(주조)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이밍(제작)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀘스트(의뢰)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐험(주조아이템 얻기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모험(제작 부가 아이템)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀴즈(제작 레시피)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 만날 때마다 일정 수치 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완주 시 -10, 사망 시 -30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10번</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100번</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1번 클리어시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전직에 필요한 5%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20번</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>난이도 &gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2723,6 +2760,447 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="49"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="49"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="49"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="49"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="49"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="49"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="49"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="49"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="49"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="49"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="49"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="49"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="49"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="49"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="49"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" s="49"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="49"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="49"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="49"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="49"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="49"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -2889,7 +3367,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2928,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>245</v>
@@ -2937,7 +3415,7 @@
         <v>252</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G2" s="23">
         <v>50</v>
@@ -2951,13 +3429,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>245</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>200</v>
@@ -2974,7 +3452,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>245</v>
@@ -2983,7 +3461,7 @@
         <v>251</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G4" s="23">
         <v>50</v>
@@ -2997,7 +3475,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>253</v>
@@ -3012,24 +3490,24 @@
         <v>50</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>250</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G6" s="23">
         <v>50</v>
@@ -3043,7 +3521,7 @@
         <v>248</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>254</v>
@@ -3063,7 +3541,7 @@
         <v>249</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>255</v>
@@ -3072,7 +3550,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G8" s="23">
         <v>50</v>
@@ -3083,16 +3561,16 @@
         <v>250</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>256</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F9" s="44" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G9" s="23">
         <v>100</v>
@@ -3103,7 +3581,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>257</v>
@@ -3112,7 +3590,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G10" s="23">
         <v>100</v>
@@ -3127,17 +3605,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="15"/>
-    <col min="2" max="2" width="9.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="9" style="15"/>
+    <col min="2" max="3" width="12.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="15"/>
     <col min="9" max="9" width="30.375" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.75" style="15" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="15"/>
@@ -3148,10 +3630,10 @@
         <v>264</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
@@ -3159,10 +3641,10 @@
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
       <c r="I1" s="37" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3170,26 +3652,26 @@
         <v>2</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>93</v>
+        <v>446</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>265</v>
+        <v>447</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>266</v>
+        <v>449</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>267</v>
+        <v>448</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>268</v>
+        <v>450</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J2" s="39"/>
     </row>
@@ -3198,26 +3680,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>358</v>
+        <v>447</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>263</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>271</v>
-      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J3" s="39"/>
     </row>
@@ -3226,16 +3704,16 @@
         <v>34</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F4" s="39" t="s">
         <v>107</v>
@@ -3244,75 +3722,75 @@
         <v>178</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>262</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>178</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>178</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3329,9 +3807,93 @@
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>451</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>452</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E15" s="15">
+        <v>100</v>
+      </c>
+      <c r="F15" s="15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E16" s="15">
+        <v>1000</v>
+      </c>
+      <c r="F16" s="15">
+        <v>10</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="G17" s="15">
+        <v>100</v>
+      </c>
+      <c r="H17" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G18" s="15">
+        <v>100</v>
+      </c>
+      <c r="H18" s="15">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="C1:H1"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B12:J12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3343,7 +3905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF524D-E86E-4617-8759-56910C557665}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3409,7 +3971,7 @@
         <v>202</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>204</v>
@@ -3430,7 +3992,7 @@
         <v>219</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K2" s="30" t="s">
         <v>263</v>
@@ -3445,7 +4007,7 @@
         <v>217</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3453,36 +4015,36 @@
         <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="2"/>
       <c r="J3" s="43" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
       <c r="O3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3490,36 +4052,36 @@
         <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
       <c r="J4" s="30" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3527,7 +4089,7 @@
         <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>100</v>
@@ -3536,25 +4098,25 @@
         <v>3</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="30" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="K5" s="30" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3562,10 +4124,10 @@
         <v>208</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
@@ -3581,7 +4143,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3590,7 +4152,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
@@ -3653,7 +4215,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3929,329 +4491,329 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E2" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D9" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E9" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D10" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E10" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D11" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E11" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B19" s="29"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B20" s="29"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B21" s="29"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B28" s="29"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B32" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B33" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="29" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="29" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -4261,11 +4823,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388325C-0B46-44CF-8403-062AA349A905}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4285,12 +4862,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C1" s="46"/>
       <c r="D1" s="46"/>
       <c r="E1" s="47" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F1" s="47"/>
       <c r="G1" s="47"/>
@@ -4303,14 +4880,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="30" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -4323,12 +4900,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -4341,12 +4918,12 @@
         <v>34</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
@@ -4356,15 +4933,15 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
@@ -4374,7 +4951,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -4543,7 +5120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -4560,39 +5137,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -4600,47 +5177,47 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D3" s="29">
         <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D4" s="29">
         <v>4</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D5" s="29">
         <v>5</v>
@@ -4679,11 +5256,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -5343,445 +5920,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="49"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="49"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="49"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="49"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="49"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="49"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="49"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="49"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="D28" s="49"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>149</v>
-      </c>
-      <c r="B30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="49"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B31" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="49"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" t="s">
-        <v>157</v>
-      </c>
-      <c r="C32" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="49"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="49"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="D34" s="49"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" s="49"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" t="s">
-        <v>162</v>
-      </c>
-      <c r="C36" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="D36" s="49"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="D37" s="49"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="49"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39" t="s">
-        <v>162</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="D39" s="49"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>170</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="D40" s="49"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>175</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="49"/>
-    </row>
-  </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
mod FoundThings.csv mod FoundryRecipe.csv mod ManufactureRecipe.csv
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBDFED8-75F2-45E4-9FD2-75C7C70ED619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C0B750-3542-4340-A325-4DABB2142D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="497">
   <si>
     <t>직업</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1879,6 +1879,156 @@
   </si>
   <si>
     <t>난이도 &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KorName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EngName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낡은가죽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낡은 뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나뭇가지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백금괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가죽손잡이검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뼈손잡이검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100번두드린검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldsword</t>
+  </si>
+  <si>
+    <t>oldarmor</t>
+  </si>
+  <si>
+    <t>다듬은 뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지푸라기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누군가의갈비뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마력으로 엮은 지푸라기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뼈장식검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은도금검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금도금검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짚무늬검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뼈 활</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낡은 창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낡은 천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다듬은 나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 실</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2209,6 +2359,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2216,9 +2369,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2780,10 +2930,10 @@
       <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="49"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2792,10 +2942,10 @@
       <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2804,10 +2954,10 @@
       <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2816,10 +2966,10 @@
       <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2828,10 +2978,10 @@
       <c r="B5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2909,7 +3059,7 @@
       <c r="C14" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2918,19 +3068,19 @@
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="46"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="46"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -2939,8 +3089,8 @@
       <c r="B17" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -2949,10 +3099,10 @@
       <c r="B19" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="49"/>
+      <c r="D19" s="46"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2961,10 +3111,10 @@
       <c r="B20" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="D20" s="46"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -2973,28 +3123,28 @@
       <c r="B21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="49"/>
+      <c r="D21" s="46"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="D22" s="46"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -3003,19 +3153,19 @@
       <c r="B25" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="46"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="49"/>
+      <c r="D26" s="46"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -3024,19 +3174,19 @@
       <c r="B27" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="49"/>
+      <c r="D27" s="46"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="46"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -3045,10 +3195,10 @@
       <c r="B30" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="49"/>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -3057,10 +3207,10 @@
       <c r="B31" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="49"/>
+      <c r="D31" s="46"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -3069,37 +3219,37 @@
       <c r="B32" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="49"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="D33" s="49"/>
+      <c r="D33" s="46"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="49"/>
+      <c r="D34" s="46"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="46"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -3108,28 +3258,28 @@
       <c r="B36" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="49"/>
+      <c r="D36" s="46"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="49"/>
+      <c r="D37" s="46"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="D38" s="49"/>
+      <c r="D38" s="46"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -3138,42 +3288,38 @@
       <c r="B39" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="49"/>
+      <c r="D39" s="46"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>170</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="49"/>
+      <c r="D40" s="46"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="49"/>
+      <c r="D41" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -3186,13 +3332,17 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3607,7 +3757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G3"/>
     </sheetView>
   </sheetViews>
@@ -3811,33 +3961,33 @@
       <c r="A11" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="46" t="s">
         <v>451</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="46" t="s">
         <v>452</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E15" s="15">
@@ -4484,7 +4634,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4667,7 +4817,9 @@
       <c r="A19" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="29" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -4824,14 +4976,245 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388325C-0B46-44CF-8403-062AA349A905}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1300</v>
+      </c>
+      <c r="B4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1600</v>
+      </c>
+      <c r="B5" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1601</v>
+      </c>
+      <c r="B6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1602</v>
+      </c>
+      <c r="B7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1603</v>
+      </c>
+      <c r="B8" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1604</v>
+      </c>
+      <c r="B9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>2001</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="29">
+        <v>2100</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
+        <v>1201</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="29">
+        <v>1500</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>1501</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>484</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
+        <v>486</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>488</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1700</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1301</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1400</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1701</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4861,19 +5244,19 @@
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48" t="s">
         <v>350</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -5276,10 +5659,10 @@
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
@@ -5520,10 +5903,10 @@
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="48"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
add SubQuestListNumber.csv mod codes
</commit_message>
<xml_diff>
--- a/Excel/Re-born.xlsx
+++ b/Excel/Re-born.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityR\Reborn\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C0B750-3542-4340-A325-4DABB2142D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AE94F8-9696-4747-B85A-F80618808FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시놉시스" sheetId="2" r:id="rId1"/>
@@ -1558,14 +1558,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대장간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>주민센터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2029,6 +2021,14 @@
   </si>
   <si>
     <t>평범한 실</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대장장이길드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모험가길드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3313,13 +3313,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -3332,17 +3336,13 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3700,7 +3700,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G8" s="23">
         <v>50</v>
@@ -3717,10 +3717,10 @@
         <v>256</v>
       </c>
       <c r="E9" s="44" t="s">
+        <v>438</v>
+      </c>
+      <c r="F9" s="44" t="s">
         <v>440</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>442</v>
       </c>
       <c r="G9" s="23">
         <v>100</v>
@@ -3740,7 +3740,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G10" s="23">
         <v>100</v>
@@ -3802,22 +3802,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="39" t="s">
+        <v>444</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>445</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>446</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>449</v>
-      </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="39" t="s">
         <v>448</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>450</v>
-      </c>
       <c r="G2" s="39" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39" t="s">
@@ -3830,7 +3830,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>263</v>
@@ -3962,7 +3962,7 @@
         <v>266</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C11" s="46"/>
       <c r="D11" s="46"/>
@@ -3978,7 +3978,7 @@
         <v>263</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
@@ -3997,7 +3997,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -4008,21 +4008,21 @@
         <v>10</v>
       </c>
       <c r="G16" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="J16" s="15" t="s">
         <v>455</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G17" s="15">
         <v>100</v>
@@ -4055,8 +4055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF524D-E86E-4617-8759-56910C557665}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4157,7 +4157,7 @@
         <v>217</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4165,16 +4165,16 @@
         <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>378</v>
+        <v>495</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>372</v>
       </c>
       <c r="E3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>373</v>
@@ -4185,16 +4185,16 @@
       <c r="H3" s="30"/>
       <c r="I3" s="2"/>
       <c r="J3" s="43" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
       <c r="O3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -4202,22 +4202,22 @@
         <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>379</v>
+        <v>496</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -4231,7 +4231,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -4239,7 +4239,7 @@
         <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>100</v>
@@ -4248,25 +4248,25 @@
         <v>3</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K5" s="30" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4274,10 +4274,10 @@
         <v>208</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
@@ -4293,7 +4293,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
@@ -4365,7 +4365,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4655,24 +4655,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
         <v>413</v>
       </c>
-      <c r="B2" t="s">
-        <v>415</v>
-      </c>
       <c r="D2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D3" t="s">
         <v>301</v>
@@ -4683,10 +4683,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D4" t="s">
         <v>315</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D5" t="s">
         <v>333</v>
@@ -4708,7 +4708,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D6" t="s">
         <v>348</v>
@@ -4716,45 +4716,45 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D9" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D10" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -4810,7 +4810,7 @@
         <v>310</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4818,7 +4818,7 @@
         <v>311</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4976,10 +4976,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388325C-0B46-44CF-8403-062AA349A905}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4992,231 +4992,264 @@
         <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="29">
+        <v>1100</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>459</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="29">
+        <v>1200</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1100</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" s="29"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
+        <v>1201</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="C4" s="29"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="29">
+        <v>1300</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1300</v>
-      </c>
-      <c r="B4" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1600</v>
-      </c>
-      <c r="B5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1601</v>
-      </c>
-      <c r="B6" t="s">
-        <v>466</v>
-      </c>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1602</v>
-      </c>
-      <c r="B7" t="s">
-        <v>465</v>
-      </c>
+      <c r="A7" s="29">
+        <v>1301</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>492</v>
+      </c>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1603</v>
-      </c>
-      <c r="B8" t="s">
-        <v>467</v>
-      </c>
+      <c r="A8" s="29">
+        <v>1400</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1604</v>
-      </c>
-      <c r="B9" t="s">
-        <v>468</v>
-      </c>
+      <c r="A9" s="29">
+        <v>1500</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
-        <v>2001</v>
+        <v>1501</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>469</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>407</v>
+      <c r="A11" s="29">
+        <v>1600</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>470</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>471</v>
+      <c r="A12" s="29">
+        <v>1601</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>472</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
-        <v>2000</v>
+        <v>1602</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>473</v>
-      </c>
+        <v>463</v>
+      </c>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
-        <v>2100</v>
+        <v>1603</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>474</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
-        <v>1201</v>
+        <v>1604</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>475</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>477</v>
+        <v>491</v>
+      </c>
+      <c r="C16" s="29"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="29">
+        <v>1701</v>
       </c>
       <c r="B17" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="C17" s="29"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>2000</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="29">
+        <v>2001</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="C19" s="29"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C20" s="29"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="C21" s="29"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="29">
-        <v>1501</v>
-      </c>
-      <c r="B18" s="29" t="s">
+      <c r="B22" s="29" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="C22" s="29"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
         <v>480</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B23" s="29" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B24" s="29" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="C24" s="29"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
         <v>484</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B25" s="29" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="C25" s="29"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
         <v>486</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B26" s="29" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="C26" s="29"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B27" s="29" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
-        <v>490</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1700</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1301</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>1400</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>1701</v>
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="29">
+        <v>2100</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>495</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="C28" s="29"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="29"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C28">
+    <sortCondition ref="A2:A28"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5520,39 +5553,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>394</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>412</v>
-      </c>
       <c r="E2" s="29" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -5560,47 +5593,47 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D3" s="29">
         <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D4" s="29">
         <v>4</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D5" s="29">
         <v>5</v>

</xml_diff>